<commit_message>
test HTML template report
</commit_message>
<xml_diff>
--- a/script/税务云-正式环境fapiao/2.首页/首页.xlsx
+++ b/script/税务云-正式环境fapiao/2.首页/首页.xlsx
@@ -296,10 +296,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -316,6 +316,22 @@
       <charset val="134"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
@@ -324,16 +340,100 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -345,78 +445,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -431,36 +461,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -487,19 +487,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -511,157 +631,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -672,6 +672,32 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -690,26 +716,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,7 +744,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -741,34 +752,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="double">
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="double">
+      <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="double">
+      <top style="thin">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="double">
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -780,149 +780,149 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -945,9 +945,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
@@ -1317,7 +1314,7 @@
   <dimension ref="A1:R42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1351,9 +1348,9 @@
       <c r="F2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="16"/>
+      <c r="P2" s="14"/>
+      <c r="Q2" s="14"/>
+      <c r="R2" s="15"/>
     </row>
     <row r="3" s="1" customFormat="1" ht="14.25" spans="1:18">
       <c r="A3" s="5" t="s">
@@ -1368,9 +1365,9 @@
       <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="15"/>
-      <c r="Q3" s="15"/>
-      <c r="R3" s="16"/>
+      <c r="P3" s="14"/>
+      <c r="Q3" s="14"/>
+      <c r="R3" s="15"/>
     </row>
     <row r="4" s="1" customFormat="1" ht="14.25" spans="1:18">
       <c r="A4" s="5" t="s">
@@ -1385,9 +1382,9 @@
       <c r="F4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P4" s="15"/>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="16"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="14"/>
+      <c r="R4" s="15"/>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="5" t="s">
@@ -1458,7 +1455,6 @@
       <c r="C9" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E9" s="10"/>
       <c r="F9" s="2" t="s">
         <v>20</v>
       </c>
@@ -1473,7 +1469,6 @@
       <c r="C10" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="10"/>
       <c r="F10" s="2" t="s">
         <v>22</v>
       </c>
@@ -1516,7 +1511,6 @@
       <c r="C13" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="10"/>
       <c r="F13" s="2" t="s">
         <v>20</v>
       </c>
@@ -1531,7 +1525,6 @@
       <c r="C14" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="E14" s="10"/>
       <c r="F14" s="2" t="s">
         <v>22</v>
       </c>
@@ -1630,7 +1623,7 @@
       <c r="C21" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="D21" s="10" t="s">
         <v>39</v>
       </c>
       <c r="F21" s="1" t="s">
@@ -1647,7 +1640,7 @@
       <c r="C22" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D22" s="12"/>
+      <c r="D22" s="11"/>
       <c r="E22" s="4" t="s">
         <v>42</v>
       </c>
@@ -1665,7 +1658,7 @@
       <c r="C23" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="D23" s="11" t="s">
+      <c r="D23" s="10" t="s">
         <v>43</v>
       </c>
       <c r="F23" s="1" t="s">
@@ -1682,7 +1675,7 @@
       <c r="C24" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="12"/>
+      <c r="D24" s="11"/>
       <c r="E24" s="4" t="s">
         <v>42</v>
       </c>
@@ -1861,13 +1854,13 @@
       </c>
     </row>
     <row r="37" s="3" customFormat="1" spans="1:6">
-      <c r="A37" s="13"/>
-      <c r="B37" s="14"/>
-      <c r="C37" s="14"/>
+      <c r="A37" s="12"/>
+      <c r="B37" s="13"/>
+      <c r="C37" s="13"/>
       <c r="E37" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F37" s="14"/>
+      <c r="F37" s="13"/>
     </row>
     <row r="38" spans="1:6">
       <c r="A38" s="5" t="s">

</xml_diff>